<commit_message>
Updated data, times and result files
- Added a measurement that starts and ends on a different day,
- The result file now includes the start and end gas concentrations.
</commit_message>
<xml_diff>
--- a/tests/times_example.xlsx
+++ b/tests/times_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t xml:space="preserve">J6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:58:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:02:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J7</t>
   </si>
 </sst>
 </file>
@@ -264,7 +273,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -275,7 +284,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="16.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="24.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,11 +461,28 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
+      <c r="A8" s="3" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>17.2</v>
+      </c>
       <c r="G8" s="5"/>
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>

</xml_diff>